<commit_message>
pulling in ayfp data
</commit_message>
<xml_diff>
--- a/ay/Data/CleanedAYData.xlsx
+++ b/ay/Data/CleanedAYData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mabellezhang/AY_Data_App/AYData/ay/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0285801E-AEA1-E541-A862-1B07AB9A482E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFAC209-85E5-3847-888C-BA8D89F08AE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="460" windowWidth="23020" windowHeight="15980" activeTab="2" xr2:uid="{025A1F25-3ABF-9246-B534-6DF4141DE7DD}"/>
+    <workbookView xWindow="2080" yWindow="460" windowWidth="23020" windowHeight="15980" activeTab="3" xr2:uid="{025A1F25-3ABF-9246-B534-6DF4141DE7DD}"/>
   </bookViews>
   <sheets>
     <sheet name="AYPOP" sheetId="1" r:id="rId1"/>
     <sheet name="KLEAgeEvents" sheetId="2" r:id="rId2"/>
     <sheet name="KLEMarriage" sheetId="3" r:id="rId3"/>
+    <sheet name="AYFPUse" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="153">
   <si>
     <t>Country</t>
   </si>
@@ -360,6 +361,132 @@
   </si>
   <si>
     <t>First Birth</t>
+  </si>
+  <si>
+    <t>Source for Ever and Recent Sexual Activity; Modern &amp; Traditional Prevelance; Unmet Need; Total Demand; and Condom Use at Last Sex</t>
+  </si>
+  <si>
+    <t>Never have had sex older adolescents aged 15-19</t>
+  </si>
+  <si>
+    <t>Never have had sex older youth aged 20-24</t>
+  </si>
+  <si>
+    <t>Recent sex older adolescents aged 15-19</t>
+  </si>
+  <si>
+    <t>Recent sex older youth aged 20-24</t>
+  </si>
+  <si>
+    <t>MCPR for unmarried sexually active adolescents (15-19)**</t>
+  </si>
+  <si>
+    <t>MCPR for unmarried sexually active youth (20-24)**</t>
+  </si>
+  <si>
+    <t>MCPR for married adolescents (15-19)</t>
+  </si>
+  <si>
+    <t>MCPR for married youth (20-24)</t>
+  </si>
+  <si>
+    <t>MCPR for married adolescent and youth (15-24)</t>
+  </si>
+  <si>
+    <t>% of unmarried sexually active** older adolescents aged 15-19 using a traditional method</t>
+  </si>
+  <si>
+    <t>% of unmarried sexually active** older youth aged 20-24 using a traditional method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of married older adolescents aged 15-19 using a traditional method </t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of married older youth aged 20-24 using a traditional method </t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of married youth aged 15-24 using a traditional method </t>
+  </si>
+  <si>
+    <t>Unmet need: 15-49 sexually active – unmarried**</t>
+  </si>
+  <si>
+    <t>Unmet need: 15-19 sexually active – unmarried**</t>
+  </si>
+  <si>
+    <t>Unmet need: 20-24 sexually active – unmarried**</t>
+  </si>
+  <si>
+    <t>Unmet need: 15-24 sexually active  – unmarried**</t>
+  </si>
+  <si>
+    <t>Unmet need : 15-19 year olds – married</t>
+  </si>
+  <si>
+    <t>Unmet need: 20-24 year olds – married</t>
+  </si>
+  <si>
+    <t>Unmet need: 15-24 year olds – married</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total demand married women (15-19) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total demand married women (20-24) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total demand unmarried sexually active women (15-19) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total demand unmarried sexually active women (20-24) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condom use during last sex: 15-24 year olds </t>
+  </si>
+  <si>
+    <t>MCPR Married Women aged 15-49</t>
+  </si>
+  <si>
+    <t>Traditional Use Married Women aged 15-49</t>
+  </si>
+  <si>
+    <t>Unmet Need Married Women aged 15-49</t>
+  </si>
+  <si>
+    <t>Angola*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016 National Survey </t>
+  </si>
+  <si>
+    <t>2014 MICS</t>
+  </si>
+  <si>
+    <t>2017 MICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017 DHS </t>
+  </si>
+  <si>
+    <t>2011-12 LSIS</t>
+  </si>
+  <si>
+    <t>2015 MICS</t>
+  </si>
+  <si>
+    <t>2013-14 MICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015 AIS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011 National Survey </t>
+  </si>
+  <si>
+    <t>South Africa*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -3284,7 +3411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAB491E-2094-F44D-AF7E-6962AA6D1892}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -4565,4 +4692,4819 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5898797A-679E-714D-8621-A1181092F33B}">
+  <dimension ref="A1:AF80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" customWidth="1"/>
+    <col min="14" max="14" width="16.5" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16.83203125" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="14.83203125" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" customWidth="1"/>
+    <col min="22" max="22" width="16.5" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" customWidth="1"/>
+    <col min="24" max="28" width="14.5" customWidth="1"/>
+    <col min="29" max="29" width="26.83203125" customWidth="1"/>
+    <col min="30" max="30" width="18.6640625" customWidth="1"/>
+    <col min="31" max="31" width="20.5" customWidth="1"/>
+    <col min="32" max="32" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" t="s">
+        <v>130</v>
+      </c>
+      <c r="W1" t="s">
+        <v>131</v>
+      </c>
+      <c r="X1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.89</v>
+      </c>
+      <c r="G2">
+        <v>0.88</v>
+      </c>
+      <c r="J2">
+        <v>5.9671311738109994E-2</v>
+      </c>
+      <c r="K2">
+        <v>0.15276876835194744</v>
+      </c>
+      <c r="L2">
+        <v>0.13124789993744812</v>
+      </c>
+      <c r="O2">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="P2">
+        <v>2.3E-2</v>
+      </c>
+      <c r="Q2">
+        <v>2.2000000000000002E-2</v>
+      </c>
+      <c r="V2">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="W2">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="X2">
+        <v>0.26035895046815744</v>
+      </c>
+      <c r="Y2">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="Z2">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="AD2">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="AE2">
+        <v>2.7000000000000003E-2</v>
+      </c>
+      <c r="AF2">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.04</v>
+      </c>
+      <c r="F3">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G3">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="H3">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="I3">
+        <v>0.36</v>
+      </c>
+      <c r="J3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="K3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="L3">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="M3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="N3">
+        <v>1.4E-2</v>
+      </c>
+      <c r="O3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Q3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="R3">
+        <v>0.437</v>
+      </c>
+      <c r="S3">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="T3">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="U3">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="V3">
+        <v>0.43</v>
+      </c>
+      <c r="W3">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="X3">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="Y3">
+        <f>SUM(V3,J3,O3)</f>
+        <v>0.51</v>
+      </c>
+      <c r="Z3">
+        <f>SUM(W3,K3,P3)</f>
+        <v>0.54899999999999993</v>
+      </c>
+      <c r="AA3">
+        <f>SUM(S3,H3,M3)</f>
+        <v>0.755</v>
+      </c>
+      <c r="AB3">
+        <f>SUM(T3,I3,N3)</f>
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="AD3">
+        <v>0.125</v>
+      </c>
+      <c r="AE3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AF3">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E4">
+        <v>1E-3</v>
+      </c>
+      <c r="F4">
+        <v>0.78099999999999992</v>
+      </c>
+      <c r="G4">
+        <v>0.81700000000000006</v>
+      </c>
+      <c r="J4">
+        <v>0.46740792544991078</v>
+      </c>
+      <c r="K4">
+        <v>0.54545354242868016</v>
+      </c>
+      <c r="L4">
+        <v>0.51538848979960927</v>
+      </c>
+      <c r="O4">
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="P4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="Q4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="V4">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="W4">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="X4">
+        <v>0.15672874713251961</v>
+      </c>
+      <c r="Y4">
+        <v>0.68299999999999994</v>
+      </c>
+      <c r="Z4">
+        <v>0.7390000000000001</v>
+      </c>
+      <c r="AD4">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="AE4">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AF4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="E5">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.224</v>
+      </c>
+      <c r="G5">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="H5">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="I5">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="J5">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K5">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="L5">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="M5">
+        <v>3.1E-2</v>
+      </c>
+      <c r="N5">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="O5">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="P5">
+        <v>2.7E-2</v>
+      </c>
+      <c r="Q5">
+        <v>2.3E-2</v>
+      </c>
+      <c r="R5">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="S5">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="T5">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="U5">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="V5">
+        <v>0.33</v>
+      </c>
+      <c r="W5">
+        <v>0.37</v>
+      </c>
+      <c r="X5">
+        <v>0.36</v>
+      </c>
+      <c r="Y5">
+        <f>SUM(V5,J5,O5)</f>
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="Z5">
+        <f>SUM(W5,K5,P5)</f>
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="AA5">
+        <f>SUM(S5,H5,M5)</f>
+        <v>0.88100000000000012</v>
+      </c>
+      <c r="AB5">
+        <f>SUM(T5,I5,N5)</f>
+        <v>0.78199999999999992</v>
+      </c>
+      <c r="AC5">
+        <v>0.11</v>
+      </c>
+      <c r="AD5">
+        <v>0.155</v>
+      </c>
+      <c r="AE5">
+        <v>3.1E-2</v>
+      </c>
+      <c r="AF5">
+        <v>0.32300000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H7">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="I7">
+        <v>0.751</v>
+      </c>
+      <c r="J7">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="K7">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="M7">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="N7">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="O7">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="P7">
+        <v>0.183</v>
+      </c>
+      <c r="AD7">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="AE7">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.35700000000000004</v>
+      </c>
+      <c r="F9">
+        <v>5.9000000000000004E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.41600000000000004</v>
+      </c>
+      <c r="H9">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="J9">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="K9">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="L9">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="M9">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="N9">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="O9">
+        <v>0.03</v>
+      </c>
+      <c r="P9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="Q9">
+        <v>0.04</v>
+      </c>
+      <c r="R9">
+        <v>0.34700000000000003</v>
+      </c>
+      <c r="S9">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="T9">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="U9">
+        <v>0.312</v>
+      </c>
+      <c r="V9">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="W9">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="X9">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="Y9">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="Z9">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="AA9">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="AB9">
+        <v>0.68299999999999994</v>
+      </c>
+      <c r="AC9">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="AD9">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="AE9">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="AF9">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10">
+        <v>0.82900000000000007</v>
+      </c>
+      <c r="E10">
+        <v>0.35200000000000004</v>
+      </c>
+      <c r="F10">
+        <v>0.124</v>
+      </c>
+      <c r="G10">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.20155283153077722</v>
+      </c>
+      <c r="K10">
+        <v>0.34386504010339281</v>
+      </c>
+      <c r="L10">
+        <v>0.31578908174451198</v>
+      </c>
+      <c r="O10">
+        <v>8.900000000000001E-2</v>
+      </c>
+      <c r="P10">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="Q10">
+        <v>0.125</v>
+      </c>
+      <c r="R10">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="U10">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="V10">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="W10">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="X10">
+        <v>0.1390240118276217</v>
+      </c>
+      <c r="Y10">
+        <v>0.44</v>
+      </c>
+      <c r="Z10">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="AD10">
+        <v>0.38799999999999996</v>
+      </c>
+      <c r="AE10">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AF10">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>143</v>
+      </c>
+      <c r="J11">
+        <v>9.3000000000000013E-2</v>
+      </c>
+      <c r="K11">
+        <v>0.15</v>
+      </c>
+      <c r="L11">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="O11">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="P11">
+        <v>0.18899999999999997</v>
+      </c>
+      <c r="Q11">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="V11">
+        <v>0.16</v>
+      </c>
+      <c r="W11">
+        <v>0.159</v>
+      </c>
+      <c r="X11" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y11">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="Z11">
+        <v>0.47</v>
+      </c>
+      <c r="AA11">
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="AB11">
+        <v>0.88</v>
+      </c>
+      <c r="AD11">
+        <v>0.16131999999999999</v>
+      </c>
+      <c r="AE11">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AF11">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="E13">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.38</v>
+      </c>
+      <c r="G13">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="J13">
+        <v>2.2544368259844252E-2</v>
+      </c>
+      <c r="K13">
+        <v>3.4538318396761934E-2</v>
+      </c>
+      <c r="L13">
+        <v>2.9901261340059673E-2</v>
+      </c>
+      <c r="M13">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="N13">
+        <v>2.2000000000000002E-2</v>
+      </c>
+      <c r="O13">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="P13">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="Q13">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="R13">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="S13">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="T13">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="U13">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="V13">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="W13">
+        <v>0.249</v>
+      </c>
+      <c r="X13">
+        <v>0.24090806828542832</v>
+      </c>
+      <c r="Y13">
+        <v>0.254</v>
+      </c>
+      <c r="Z13">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="AA13">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="AB13">
+        <v>0.81099999999999994</v>
+      </c>
+      <c r="AC13">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="AD13">
+        <v>0.05</v>
+      </c>
+      <c r="AE13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AF13">
+        <v>0.22899999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="E14">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F14">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G14">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="J14">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="K14">
+        <v>0.14300000000000002</v>
+      </c>
+      <c r="L14">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="N14">
+        <v>0.315</v>
+      </c>
+      <c r="O14">
+        <v>6.2E-2</v>
+      </c>
+      <c r="P14">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="Q14">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="R14">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="T14">
+        <v>0.34</v>
+      </c>
+      <c r="U14">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="V14">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="W14">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="X14">
+        <v>0.442</v>
+      </c>
+      <c r="Y14">
+        <v>0.67</v>
+      </c>
+      <c r="Z14">
+        <v>0.62</v>
+      </c>
+      <c r="AB14">
+        <v>0.99</v>
+      </c>
+      <c r="AD14">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AE14">
+        <v>5.2000000000000005E-2</v>
+      </c>
+      <c r="AF14">
+        <v>0.32299999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15">
+        <v>0.36</v>
+      </c>
+      <c r="E15">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="G15">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="H15">
+        <v>0.443</v>
+      </c>
+      <c r="I15">
+        <v>0.502</v>
+      </c>
+      <c r="J15">
+        <v>0.26348794602400655</v>
+      </c>
+      <c r="K15">
+        <v>0.23023498457953376</v>
+      </c>
+      <c r="L15">
+        <v>0.23941001824042091</v>
+      </c>
+      <c r="M15">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="N15">
+        <v>0.251</v>
+      </c>
+      <c r="O15">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="P15">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="Q15">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="R15">
+        <v>0.156</v>
+      </c>
+      <c r="S15">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="T15">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="U15">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="V15">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="W15">
+        <v>0.23199999999999998</v>
+      </c>
+      <c r="X15">
+        <v>0.26362684596218566</v>
+      </c>
+      <c r="Y15">
+        <v>0.71</v>
+      </c>
+      <c r="Z15">
+        <v>0.69</v>
+      </c>
+      <c r="AA15">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="AB15">
+        <v>0.92299999999999993</v>
+      </c>
+      <c r="AC15">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="AD15">
+        <v>0.2</v>
+      </c>
+      <c r="AE15">
+        <v>0.247</v>
+      </c>
+      <c r="AF15">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16">
+        <v>0.432</v>
+      </c>
+      <c r="E16">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.17749999999999999</v>
+      </c>
+      <c r="G16">
+        <v>0.34685359999999998</v>
+      </c>
+      <c r="H16">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="I16">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="J16">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="K16">
+        <v>0.1135</v>
+      </c>
+      <c r="L16">
+        <v>0.10249108922664631</v>
+      </c>
+      <c r="M16">
+        <v>1.9635099999999999E-2</v>
+      </c>
+      <c r="N16">
+        <v>3.8625949999999999E-2</v>
+      </c>
+      <c r="O16">
+        <v>3.667511E-3</v>
+      </c>
+      <c r="P16">
+        <v>1.11082E-2</v>
+      </c>
+      <c r="Q16">
+        <v>9.12228E-3</v>
+      </c>
+      <c r="V16">
+        <v>0.311</v>
+      </c>
+      <c r="W16">
+        <v>0.35</v>
+      </c>
+      <c r="Y16">
+        <f>SUM(V16,J16,O16)</f>
+        <v>0.38136751099999999</v>
+      </c>
+      <c r="Z16">
+        <f>SUM(W16,K16,P16)</f>
+        <v>0.47460819999999998</v>
+      </c>
+      <c r="AC16">
+        <v>0.252</v>
+      </c>
+      <c r="AD16">
+        <v>0.1376</v>
+      </c>
+      <c r="AE16">
+        <v>1.2E-2</v>
+      </c>
+      <c r="AF16">
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>144</v>
+      </c>
+      <c r="J18" t="s">
+        <v>89</v>
+      </c>
+      <c r="K18">
+        <v>0.182</v>
+      </c>
+      <c r="L18" t="s">
+        <v>89</v>
+      </c>
+      <c r="P18">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="V18" t="s">
+        <v>89</v>
+      </c>
+      <c r="W18">
+        <v>0.107</v>
+      </c>
+      <c r="X18" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD18">
+        <v>0.69</v>
+      </c>
+      <c r="AE18">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AF18">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19">
+        <v>0.47700000000000004</v>
+      </c>
+      <c r="E19">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="F19">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G19">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="H19">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="I19">
+        <v>0.252</v>
+      </c>
+      <c r="J19">
+        <v>5.4486908960099972E-2</v>
+      </c>
+      <c r="K19">
+        <v>8.2402553846181517E-2</v>
+      </c>
+      <c r="L19">
+        <v>7.4614049766422538E-2</v>
+      </c>
+      <c r="M19">
+        <v>0.19699999999999998</v>
+      </c>
+      <c r="N19">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="O19">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="P19">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="Q19">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="R19">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="S19">
+        <v>0.48200000000000004</v>
+      </c>
+      <c r="T19">
+        <v>0.41200000000000003</v>
+      </c>
+      <c r="U19">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="V19">
+        <v>0.308</v>
+      </c>
+      <c r="W19">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="X19">
+        <v>0.29690466370774721</v>
+      </c>
+      <c r="Y19">
+        <v>0.433</v>
+      </c>
+      <c r="Z19">
+        <v>0.48700000000000004</v>
+      </c>
+      <c r="AA19">
+        <v>0.92</v>
+      </c>
+      <c r="AB19">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="AC19">
+        <v>0.113</v>
+      </c>
+      <c r="AD19">
+        <v>7.8E-2</v>
+      </c>
+      <c r="AE19">
+        <v>0.126</v>
+      </c>
+      <c r="AF19">
+        <v>0.27699999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20">
+        <v>0.18884942974368363</v>
+      </c>
+      <c r="K20">
+        <v>0.40531291737065994</v>
+      </c>
+      <c r="L20">
+        <v>0.36198932009394619</v>
+      </c>
+      <c r="O20">
+        <v>1.6E-2</v>
+      </c>
+      <c r="P20">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="Q20">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="V20">
+        <v>0.09</v>
+      </c>
+      <c r="W20">
+        <v>0.11</v>
+      </c>
+      <c r="X20">
+        <v>0.10607049304347814</v>
+      </c>
+      <c r="Y20">
+        <v>0.29600000000000004</v>
+      </c>
+      <c r="Z20">
+        <v>0.53299999999999992</v>
+      </c>
+      <c r="AD20">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="AE20">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AF20">
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22">
+        <v>0.754</v>
+      </c>
+      <c r="E22">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="F22">
+        <v>0.15</v>
+      </c>
+      <c r="G22">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="H22">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="I22">
+        <v>0.47</v>
+      </c>
+      <c r="J22">
+        <v>0.31830000000000003</v>
+      </c>
+      <c r="K22">
+        <v>0.3846</v>
+      </c>
+      <c r="L22">
+        <v>0.36759999999999998</v>
+      </c>
+      <c r="M22">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="N22">
+        <v>9.3000000000000013E-2</v>
+      </c>
+      <c r="O22">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="P22">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Q22">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R22">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="S22">
+        <v>0.39799999999999996</v>
+      </c>
+      <c r="T22">
+        <v>0.317</v>
+      </c>
+      <c r="U22">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="V22">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="W22">
+        <v>0.12189999999999999</v>
+      </c>
+      <c r="X22">
+        <v>0.1852</v>
+      </c>
+      <c r="Y22">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="Z22">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="AA22">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="AB22">
+        <v>0.88</v>
+      </c>
+      <c r="AC22">
+        <v>0.39899999999999997</v>
+      </c>
+      <c r="AD22">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="AE22">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AF22">
+        <v>0.223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23">
+        <v>0.126</v>
+      </c>
+      <c r="G23">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="J23">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="K23">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="L23">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q23">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="R23">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="U23">
+        <v>0.46399999999999997</v>
+      </c>
+      <c r="V23">
+        <v>0.16899999999999998</v>
+      </c>
+      <c r="W23">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="X23">
+        <v>0.214</v>
+      </c>
+      <c r="AD23">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="AE23">
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="AF23">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="E24">
+        <v>0.129</v>
+      </c>
+      <c r="F24">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="H24">
+        <v>0.315</v>
+      </c>
+      <c r="I24">
+        <v>0.35100000000000003</v>
+      </c>
+      <c r="J24">
+        <v>0.16680868748698507</v>
+      </c>
+      <c r="K24">
+        <v>0.24750102346862071</v>
+      </c>
+      <c r="L24">
+        <v>0.23567136657543172</v>
+      </c>
+      <c r="M24">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="N24">
+        <v>0.18100000000000002</v>
+      </c>
+      <c r="O24">
+        <v>1.9E-2</v>
+      </c>
+      <c r="P24">
+        <v>4.7E-2</v>
+      </c>
+      <c r="Q24">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="R24">
+        <v>0.42200000000000004</v>
+      </c>
+      <c r="S24">
+        <v>0.505</v>
+      </c>
+      <c r="T24">
+        <v>0.38799999999999996</v>
+      </c>
+      <c r="U24">
+        <v>0.43799999999999994</v>
+      </c>
+      <c r="V24">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="W24">
+        <v>0.34</v>
+      </c>
+      <c r="X24">
+        <v>0.36433949204293298</v>
+      </c>
+      <c r="Y24">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="Z24">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="AA24">
+        <v>0.94200000000000006</v>
+      </c>
+      <c r="AB24">
+        <v>0.92299999999999993</v>
+      </c>
+      <c r="AC24">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AD24">
+        <v>0.222</v>
+      </c>
+      <c r="AE24">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AF24">
+        <v>0.29899999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25">
+        <v>0.106</v>
+      </c>
+      <c r="K25">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="O25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P25">
+        <v>1E-3</v>
+      </c>
+      <c r="V25">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="W25">
+        <v>0.2</v>
+      </c>
+      <c r="Y25">
+        <f>SUM(V25,J25,O25)</f>
+        <v>0.31</v>
+      </c>
+      <c r="Z25">
+        <f>SUM(W25,K25,P25)</f>
+        <v>0.318</v>
+      </c>
+      <c r="AD25">
+        <v>0.109</v>
+      </c>
+      <c r="AE25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AF25">
+        <v>0.221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26">
+        <v>0.32</v>
+      </c>
+      <c r="E26">
+        <v>0.2858</v>
+      </c>
+      <c r="F26">
+        <v>0.1389</v>
+      </c>
+      <c r="G26">
+        <v>0.24</v>
+      </c>
+      <c r="H26">
+        <v>0.55777155</v>
+      </c>
+      <c r="I26">
+        <v>0.68939655</v>
+      </c>
+      <c r="J26">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="K26">
+        <v>0.1</v>
+      </c>
+      <c r="L26">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="M26">
+        <v>5.8453369999999998E-2</v>
+      </c>
+      <c r="N26">
+        <v>4.0034739999999999E-2</v>
+      </c>
+      <c r="O26">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P26">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q26">
+        <v>1.2551405999999999E-2</v>
+      </c>
+      <c r="V26">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="W26">
+        <v>0.23</v>
+      </c>
+      <c r="Y26">
+        <f>SUM(V26,J26,O26)</f>
+        <v>0.36</v>
+      </c>
+      <c r="Z26">
+        <f>SUM(W26,K26,P26)</f>
+        <v>0.34500000000000003</v>
+      </c>
+      <c r="AC26">
+        <v>0.37</v>
+      </c>
+      <c r="AD26">
+        <v>0.14373</v>
+      </c>
+      <c r="AE26">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AF26">
+        <v>0.223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="E27">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F27">
+        <v>0.154</v>
+      </c>
+      <c r="G27">
+        <v>0.441</v>
+      </c>
+      <c r="H27">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="I27">
+        <v>0.33799999999999997</v>
+      </c>
+      <c r="J27">
+        <v>0.248</v>
+      </c>
+      <c r="K27">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="L27">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="M27">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="N27">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="O27">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P27">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q27">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="R27">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="S27">
+        <v>0.67099999999999993</v>
+      </c>
+      <c r="T27">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="U27">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="V27">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="W27">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="X27">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="Y27">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="Z27">
+        <v>0.82200000000000006</v>
+      </c>
+      <c r="AA27">
+        <v>0.97400000000000009</v>
+      </c>
+      <c r="AB27">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="AC27">
+        <v>0.46799999999999997</v>
+      </c>
+      <c r="AD27">
+        <v>0.318</v>
+      </c>
+      <c r="AE27">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AF27">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="E28">
+        <v>0.214</v>
+      </c>
+      <c r="F28">
+        <v>0.23</v>
+      </c>
+      <c r="G28">
+        <v>0.504</v>
+      </c>
+      <c r="H28">
+        <v>0.54</v>
+      </c>
+      <c r="I28">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="J28">
+        <v>0.49400928652219517</v>
+      </c>
+      <c r="K28">
+        <v>0.61470548400473657</v>
+      </c>
+      <c r="L28">
+        <v>0.57201269751480399</v>
+      </c>
+      <c r="M28">
+        <v>0.157</v>
+      </c>
+      <c r="N28">
+        <v>0.11900000000000001</v>
+      </c>
+      <c r="O28">
+        <v>6.2E-2</v>
+      </c>
+      <c r="P28">
+        <v>7.8E-2</v>
+      </c>
+      <c r="Q28">
+        <v>7.2000000000000008E-2</v>
+      </c>
+      <c r="R28">
+        <v>0.11900000000000001</v>
+      </c>
+      <c r="S28">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="T28">
+        <v>0.152</v>
+      </c>
+      <c r="U28">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="V28">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="W28">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="X28">
+        <v>0.14732584936835308</v>
+      </c>
+      <c r="Y28">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="Z28">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="AA28">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="AB28">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="AC28">
+        <v>0.38</v>
+      </c>
+      <c r="AD28">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="AE28">
+        <v>9.3000000000000013E-2</v>
+      </c>
+      <c r="AF28">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="E29">
+        <v>0.33</v>
+      </c>
+      <c r="F29">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G29">
+        <v>0.42200000000000004</v>
+      </c>
+      <c r="I29">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="J29">
+        <v>9.9599999999999994E-2</v>
+      </c>
+      <c r="K29">
+        <v>0.2356</v>
+      </c>
+      <c r="L29">
+        <v>0.21010000000000001</v>
+      </c>
+      <c r="O29">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="P29">
+        <v>5.3600000000000002E-2</v>
+      </c>
+      <c r="Q29">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="R29">
+        <v>0.185</v>
+      </c>
+      <c r="S29">
+        <v>0.22899999999999998</v>
+      </c>
+      <c r="T29">
+        <v>0.10800000000000001</v>
+      </c>
+      <c r="U29">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="V29">
+        <v>0.222</v>
+      </c>
+      <c r="W29">
+        <v>0.223</v>
+      </c>
+      <c r="X29">
+        <v>0.222</v>
+      </c>
+      <c r="Y29">
+        <v>0.37</v>
+      </c>
+      <c r="Z29">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="AA29">
+        <v>0.34600000000000003</v>
+      </c>
+      <c r="AB29">
+        <v>0.54299999999999993</v>
+      </c>
+      <c r="AC29">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="AD29">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="AE29">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="AF29">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>145</v>
+      </c>
+      <c r="J30">
+        <v>0.438</v>
+      </c>
+      <c r="K30">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="O30">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="P30">
+        <v>3.9E-2</v>
+      </c>
+      <c r="V30">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="W30">
+        <v>9.4E-2</v>
+      </c>
+      <c r="Y30">
+        <f>SUM(V30,J30,O30)</f>
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="Z30">
+        <f>SUM(W30,K30,P30)</f>
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="AD30">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="AE30">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="AF30">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>95</v>
+      </c>
+      <c r="J31">
+        <v>0.155</v>
+      </c>
+      <c r="K31">
+        <v>0.19</v>
+      </c>
+      <c r="L31">
+        <v>0.34179999999999999</v>
+      </c>
+      <c r="O31">
+        <v>0.06</v>
+      </c>
+      <c r="P31">
+        <v>0.158</v>
+      </c>
+      <c r="Q31">
+        <v>0.12948999999999999</v>
+      </c>
+      <c r="V31">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="W31">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="Y31">
+        <f>SUM(V31,J31,O31)</f>
+        <v>0.35400000000000004</v>
+      </c>
+      <c r="Z31">
+        <f>SUM(W31,K31,P31)</f>
+        <v>0.496</v>
+      </c>
+      <c r="AD31">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="AE31">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="AF31">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="E32">
+        <v>0.105</v>
+      </c>
+      <c r="F32">
+        <v>0.114</v>
+      </c>
+      <c r="G32">
+        <v>0.49200000000000005</v>
+      </c>
+      <c r="H32">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="I32">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="J32">
+        <v>0.36793043159587502</v>
+      </c>
+      <c r="K32">
+        <v>0.49831303457737147</v>
+      </c>
+      <c r="L32">
+        <v>0.47465047717583514</v>
+      </c>
+      <c r="M32">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="N32">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="O32">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="P32">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="Q32">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="R32">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="S32">
+        <v>0.439</v>
+      </c>
+      <c r="T32">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="U32">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="V32">
+        <v>0.23</v>
+      </c>
+      <c r="W32">
+        <v>0.18899999999999997</v>
+      </c>
+      <c r="X32">
+        <v>0.19597806993386951</v>
+      </c>
+      <c r="Y32">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="Z32">
+        <v>0.71900000000000008</v>
+      </c>
+      <c r="AA32">
+        <v>0.93900000000000006</v>
+      </c>
+      <c r="AB32">
+        <v>0.93299999999999994</v>
+      </c>
+      <c r="AC32">
+        <v>0.375</v>
+      </c>
+      <c r="AD32">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="AE32">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AF32">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="E33">
+        <v>0.35600000000000004</v>
+      </c>
+      <c r="F33">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G33">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="J33">
+        <v>5.1508981970041286E-2</v>
+      </c>
+      <c r="K33">
+        <v>0.19507020071789991</v>
+      </c>
+      <c r="L33">
+        <v>0.17358045179044429</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>2.3E-2</v>
+      </c>
+      <c r="Q33">
+        <v>1.9E-2</v>
+      </c>
+      <c r="R33">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="V33">
+        <v>0.21165780632660486</v>
+      </c>
+      <c r="W33">
+        <v>0.21165780632660486</v>
+      </c>
+      <c r="X33">
+        <v>0.21165780632660486</v>
+      </c>
+      <c r="Y33">
+        <v>0.14800000000000002</v>
+      </c>
+      <c r="Z33">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="AD33">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="AE33">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="AF33">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>146</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0.23616000000000001</v>
+      </c>
+      <c r="K34">
+        <v>0.36406999999999995</v>
+      </c>
+      <c r="L34">
+        <v>0.32484000000000002</v>
+      </c>
+      <c r="O34">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="P34">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="Q34">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="W34">
+        <v>0.21</v>
+      </c>
+      <c r="X34">
+        <v>0.215</v>
+      </c>
+      <c r="AD34">
+        <v>0.42724000000000001</v>
+      </c>
+      <c r="AE34">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="AF34">
+        <v>0.19900000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="E35">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="F35">
+        <v>0.129</v>
+      </c>
+      <c r="G35">
+        <v>0.37</v>
+      </c>
+      <c r="H35">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="I35">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="J35">
+        <v>0.3527383983152817</v>
+      </c>
+      <c r="K35">
+        <v>0.5736949875986882</v>
+      </c>
+      <c r="L35">
+        <v>0.51472563521935844</v>
+      </c>
+      <c r="M35">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="N35">
+        <v>0.03</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q35">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="R35">
+        <v>0.20199999999999999</v>
+      </c>
+      <c r="S35">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="T35">
+        <v>0.26</v>
+      </c>
+      <c r="U35">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="V35">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="W35">
+        <v>0.215</v>
+      </c>
+      <c r="X35">
+        <v>0.23439539961957437</v>
+      </c>
+      <c r="Y35">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="Z35">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="AA35">
+        <v>0.995</v>
+      </c>
+      <c r="AB35">
+        <v>0.96200000000000008</v>
+      </c>
+      <c r="AC35">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="AD35">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="AE35">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AF35">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36">
+        <v>0.3</v>
+      </c>
+      <c r="E36">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="F36">
+        <v>0.38</v>
+      </c>
+      <c r="G36">
+        <v>0.59</v>
+      </c>
+      <c r="H36">
+        <v>0.25</v>
+      </c>
+      <c r="I36">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="J36">
+        <v>0.13204288184186525</v>
+      </c>
+      <c r="K36">
+        <v>0.22528746281763726</v>
+      </c>
+      <c r="L36">
+        <v>0.20128964013914749</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q36">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="R36">
+        <v>0.46299999999999997</v>
+      </c>
+      <c r="S36">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="T36">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="U36">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="V36">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="W36">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="X36">
+        <v>0.40671296877910079</v>
+      </c>
+      <c r="Y36">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="Z36">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="AA36">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="AB36">
+        <v>0.878</v>
+      </c>
+      <c r="AD36">
+        <v>0.191</v>
+      </c>
+      <c r="AE36">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AF36">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38">
+        <v>0.48100000000000004</v>
+      </c>
+      <c r="E38">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F38">
+        <v>0.22699999999999998</v>
+      </c>
+      <c r="G38">
+        <v>0.57100000000000006</v>
+      </c>
+      <c r="H38">
+        <v>0.32</v>
+      </c>
+      <c r="I38">
+        <v>0.43700000000000006</v>
+      </c>
+      <c r="J38">
+        <v>0.375</v>
+      </c>
+      <c r="K38">
+        <v>0.54799999999999993</v>
+      </c>
+      <c r="L38">
+        <v>0.504</v>
+      </c>
+      <c r="M38">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="N38">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O38">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P38">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Q38">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="R38">
+        <v>0.39799999999999996</v>
+      </c>
+      <c r="S38">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="T38">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="U38">
+        <v>0.45799999999999996</v>
+      </c>
+      <c r="V38">
+        <v>0.222</v>
+      </c>
+      <c r="W38">
+        <v>0.184</v>
+      </c>
+      <c r="X38">
+        <v>0.19399999999999998</v>
+      </c>
+      <c r="Y38">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="Z38">
+        <v>0.74</v>
+      </c>
+      <c r="AA38">
+        <v>0.85400000000000009</v>
+      </c>
+      <c r="AB38">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="AC38">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="AD38">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="AE38">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="AF38">
+        <v>0.187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="E39">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F39">
+        <v>0.376</v>
+      </c>
+      <c r="G39">
+        <v>0.67</v>
+      </c>
+      <c r="H39">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="I39">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="M39">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N39">
+        <v>1.4E-2</v>
+      </c>
+      <c r="R39">
+        <v>0.54799999999999993</v>
+      </c>
+      <c r="S39">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="T39">
+        <v>0.46799999999999997</v>
+      </c>
+      <c r="U39">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="V39">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="W39">
+        <v>0.245</v>
+      </c>
+      <c r="X39">
+        <v>0.24127439818091811</v>
+      </c>
+      <c r="Y39">
+        <v>0.3</v>
+      </c>
+      <c r="Z39">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="AA39">
+        <v>0.871</v>
+      </c>
+      <c r="AB39">
+        <v>0.8909999999999999</v>
+      </c>
+      <c r="AC39">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="AD39">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="AE39">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AF39">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>147</v>
+      </c>
+      <c r="J40">
+        <v>7.7350000000000002E-2</v>
+      </c>
+      <c r="K40">
+        <v>0.159384</v>
+      </c>
+      <c r="L40">
+        <v>0.13159999999999999</v>
+      </c>
+      <c r="O40">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="P40">
+        <v>1.8589999999999999E-2</v>
+      </c>
+      <c r="Q40">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="V40">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="W40">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="Y40">
+        <f>SUM(V40,J40,O40)</f>
+        <v>0.48035000000000005</v>
+      </c>
+      <c r="Z40">
+        <f>SUM(W40,K40,P40)</f>
+        <v>0.52697399999999994</v>
+      </c>
+      <c r="AD40">
+        <v>0.15640000000000001</v>
+      </c>
+      <c r="AE40">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AF40">
+        <v>0.33600000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="E41">
+        <v>0.1613</v>
+      </c>
+      <c r="F41">
+        <v>1.9854500000000001E-2</v>
+      </c>
+      <c r="G41">
+        <v>0.3344453</v>
+      </c>
+      <c r="H41">
+        <v>0.29450795000000002</v>
+      </c>
+      <c r="I41">
+        <v>0.30843367240000003</v>
+      </c>
+      <c r="J41">
+        <v>0.35472320000000002</v>
+      </c>
+      <c r="K41">
+        <v>0.36385459999999997</v>
+      </c>
+      <c r="L41">
+        <v>0.36322726999999999</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>7.0026380000000003E-3</v>
+      </c>
+      <c r="P41">
+        <v>2.4526736600000001E-2</v>
+      </c>
+      <c r="Q41">
+        <v>2.3322820000000001E-2</v>
+      </c>
+      <c r="V41">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="W41">
+        <v>0.217</v>
+      </c>
+      <c r="Y41">
+        <f>SUM(V41,J41,O41)</f>
+        <v>0.60472583800000002</v>
+      </c>
+      <c r="Z41">
+        <f>SUM(W41,K41,P41)</f>
+        <v>0.60538133660000004</v>
+      </c>
+      <c r="AC41">
+        <v>0.243998089</v>
+      </c>
+      <c r="AD41">
+        <v>0.36596448999999998</v>
+      </c>
+      <c r="AE41">
+        <v>2.2222169999999999E-2</v>
+      </c>
+      <c r="AF41">
+        <v>0.22600000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E42">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F42">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G42">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="H42">
+        <v>0.443</v>
+      </c>
+      <c r="I42">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="J42">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="K42">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="L42">
+        <v>0.214</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="O42">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="P42">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Q42">
+        <v>0.01</v>
+      </c>
+      <c r="R42">
+        <v>0.3</v>
+      </c>
+      <c r="S42">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="T42">
+        <v>0.185</v>
+      </c>
+      <c r="U42">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="V42">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="W42">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="X42">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="Y42">
+        <f>SUM(V42,J42,O42)</f>
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="Z42">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="AA42">
+        <f>SUM(S42,H42,M42)</f>
+        <v>0.80699999999999994</v>
+      </c>
+      <c r="AB42">
+        <f>SUM(T42,I42,N42)</f>
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="AD42">
+        <v>0.253</v>
+      </c>
+      <c r="AE42">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="AF42">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43">
+        <v>0.8640000000000001</v>
+      </c>
+      <c r="E43">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="F43">
+        <v>0.105</v>
+      </c>
+      <c r="G43">
+        <v>0.36</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="K43">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="L43">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O43">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P43">
+        <v>1E-3</v>
+      </c>
+      <c r="Q43">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="V43">
+        <v>0.18899999999999997</v>
+      </c>
+      <c r="W43">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="X43" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y43">
+        <v>0.72900000000000009</v>
+      </c>
+      <c r="Z43">
+        <v>0.73</v>
+      </c>
+      <c r="AD43">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="AE43">
+        <v>0.01</v>
+      </c>
+      <c r="AF43">
+        <v>0.16200000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="E44">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="F44">
+        <v>0.153</v>
+      </c>
+      <c r="G44">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0.14480000000000001</v>
+      </c>
+      <c r="K44">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="L44">
+        <v>0.2114</v>
+      </c>
+      <c r="O44">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="P44">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="Q44">
+        <v>8.2600000000000007E-2</v>
+      </c>
+      <c r="V44">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="W44">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="X44">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="Y44">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Z44">
+        <v>0.64599999999999991</v>
+      </c>
+      <c r="AD44">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="AE44">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="AF44">
+        <v>0.23699999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>150</v>
+      </c>
+      <c r="H45">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="I45">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="J45">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="K45">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="M45">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N45">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="O45">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P45">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="V45">
+        <v>0.108</v>
+      </c>
+      <c r="W45">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="Y45">
+        <f>SUM(V45,J45,O45)</f>
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="Z45">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="AD45">
+        <v>0.77</v>
+      </c>
+      <c r="AE45">
+        <v>0.03</v>
+      </c>
+      <c r="AF45">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46">
+        <v>0.37200000000000005</v>
+      </c>
+      <c r="E46">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F46">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="G46">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="J46">
+        <v>5.9165305481543876E-2</v>
+      </c>
+      <c r="K46">
+        <v>0.12644796088329852</v>
+      </c>
+      <c r="L46">
+        <v>0.10072887910339551</v>
+      </c>
+      <c r="O46">
+        <v>1E-3</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0.496</v>
+      </c>
+      <c r="V46">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="W46">
+        <v>0.184</v>
+      </c>
+      <c r="X46">
+        <v>0.16335701481168452</v>
+      </c>
+      <c r="Y46">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="Z46">
+        <v>0.33</v>
+      </c>
+      <c r="AD46">
+        <v>0.122</v>
+      </c>
+      <c r="AE46">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AF46">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>98</v>
+      </c>
+      <c r="J47">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K47">
+        <v>0.109</v>
+      </c>
+      <c r="O47">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="P47">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="V47">
+        <v>0.122</v>
+      </c>
+      <c r="W47">
+        <v>0.161</v>
+      </c>
+      <c r="Y47">
+        <f>SUM(V47,J47,O47)</f>
+        <v>0.154</v>
+      </c>
+      <c r="Z47">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="AD47">
+        <v>0.12</v>
+      </c>
+      <c r="AE47">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="AF47">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="E48">
+        <v>0.505</v>
+      </c>
+      <c r="F48">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="G48">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="J48">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K48">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="L48">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="O48">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P48">
+        <v>0.05</v>
+      </c>
+      <c r="Q48">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="V48">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="W48">
+        <v>0.186</v>
+      </c>
+      <c r="X48">
+        <v>0.184</v>
+      </c>
+      <c r="Y48">
+        <f>SUM(V48,J48,O48)</f>
+        <v>0.253</v>
+      </c>
+      <c r="Z48">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="AD48">
+        <v>0.25</v>
+      </c>
+      <c r="AE48">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="AF48">
+        <v>0.17299999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50">
+        <v>0.878</v>
+      </c>
+      <c r="E50">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="F50">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G50">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="H50">
+        <v>0.129</v>
+      </c>
+      <c r="I50">
+        <v>0.152</v>
+      </c>
+      <c r="J50">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="K50">
+        <v>0.44</v>
+      </c>
+      <c r="L50">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="M50">
+        <v>0.185</v>
+      </c>
+      <c r="N50">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="O50">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="P50">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="Q50">
+        <v>0.106</v>
+      </c>
+      <c r="R50">
+        <v>0.48700000000000004</v>
+      </c>
+      <c r="S50">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="T50">
+        <v>0.45899999999999996</v>
+      </c>
+      <c r="U50">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="V50">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="W50">
+        <v>0.184</v>
+      </c>
+      <c r="X50">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="Y50">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="Z50">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="AA50">
+        <v>0.93099999999999994</v>
+      </c>
+      <c r="AB50">
+        <v>0.878</v>
+      </c>
+      <c r="AD50">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="AE50">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AF50">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="E51">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="F51">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="G51">
+        <v>0.36700000000000005</v>
+      </c>
+      <c r="H51">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="I51">
+        <v>0.34299999999999997</v>
+      </c>
+      <c r="J51">
+        <v>0.32818947769906492</v>
+      </c>
+      <c r="K51">
+        <v>0.44318977870328119</v>
+      </c>
+      <c r="L51">
+        <v>0.43309574218883018</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P51">
+        <v>3.1E-2</v>
+      </c>
+      <c r="Q51">
+        <v>0.03</v>
+      </c>
+      <c r="R51">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="S51">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="T51">
+        <v>0.49</v>
+      </c>
+      <c r="U51">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="V51">
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="W51">
+        <v>0.14800000000000002</v>
+      </c>
+      <c r="X51">
+        <v>0.13879034914446101</v>
+      </c>
+      <c r="Y51">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="Z51">
+        <v>0.622</v>
+      </c>
+      <c r="AA51">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="AB51">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="AC51">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="AD51">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AE51">
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="AF51">
+        <v>0.18899999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52">
+        <v>0.46</v>
+      </c>
+      <c r="E52">
+        <v>6.8165000000000003E-2</v>
+      </c>
+      <c r="F52">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G52">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="H52">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="I52">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J52">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="K52">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="L52">
+        <v>0.371</v>
+      </c>
+      <c r="M52">
+        <v>5.9461630000000001E-2</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>2.4E-2</v>
+      </c>
+      <c r="P52">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="Q52">
+        <v>1.9E-2</v>
+      </c>
+      <c r="V52">
+        <v>0.42200000000000004</v>
+      </c>
+      <c r="W52">
+        <v>0.32299999999999995</v>
+      </c>
+      <c r="X52" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y52">
+        <f>SUM(V52,J52,O52)</f>
+        <v>0.72200000000000009</v>
+      </c>
+      <c r="Z52">
+        <f>SUM(W52,K52,P52)</f>
+        <v>0.749</v>
+      </c>
+      <c r="AC52">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="AD52">
+        <v>0.37391999999999997</v>
+      </c>
+      <c r="AE52">
+        <v>0.03</v>
+      </c>
+      <c r="AF52">
+        <v>0.32700000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="E53">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="F53">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="G53">
+        <v>0.36</v>
+      </c>
+      <c r="H53">
+        <v>0.23600000000000002</v>
+      </c>
+      <c r="I53">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="J53">
+        <v>0.09</v>
+      </c>
+      <c r="K53">
+        <v>0.189</v>
+      </c>
+      <c r="L53">
+        <v>0.153</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="P53">
+        <v>1.2E-2</v>
+      </c>
+      <c r="Q53">
+        <v>0.01</v>
+      </c>
+      <c r="R53">
+        <v>0.377</v>
+      </c>
+      <c r="S53">
+        <v>0.64</v>
+      </c>
+      <c r="T53">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="U53">
+        <v>0.48</v>
+      </c>
+      <c r="V53">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="W53">
+        <v>0.254</v>
+      </c>
+      <c r="X53">
+        <v>0.249</v>
+      </c>
+      <c r="Y53">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="Z53">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="AA53">
+        <v>0.87599999999999989</v>
+      </c>
+      <c r="AB53">
+        <v>0.92099999999999993</v>
+      </c>
+      <c r="AD53">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="AE53">
+        <v>1.4E-2</v>
+      </c>
+      <c r="AF53">
+        <v>0.219</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="E54">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F54">
+        <v>0.1085</v>
+      </c>
+      <c r="G54">
+        <v>0.26841759999999998</v>
+      </c>
+      <c r="H54">
+        <v>0.5397805</v>
+      </c>
+      <c r="I54">
+        <v>0.55864610000000003</v>
+      </c>
+      <c r="J54">
+        <v>0.13968839999999999</v>
+      </c>
+      <c r="K54">
+        <v>0.20164000000000001</v>
+      </c>
+      <c r="L54">
+        <v>0.18602379999999999</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>8.9084569999999998E-3</v>
+      </c>
+      <c r="O54">
+        <v>2.9162139999999999E-3</v>
+      </c>
+      <c r="P54">
+        <v>3.2776239999999998E-3</v>
+      </c>
+      <c r="Q54">
+        <v>3.18651E-3</v>
+      </c>
+      <c r="V54">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="W54">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="Y54">
+        <f>SUM(V54,J54,O54)</f>
+        <v>0.42860461399999994</v>
+      </c>
+      <c r="Z54">
+        <f>SUM(W54,K54,P54)</f>
+        <v>0.47791762400000004</v>
+      </c>
+      <c r="AA54">
+        <v>0.92299999999999993</v>
+      </c>
+      <c r="AB54">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="AC54">
+        <v>7.7954144000000003E-2</v>
+      </c>
+      <c r="AD54">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="AE54">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AF54">
+        <v>0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+      <c r="J55">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="K55">
+        <v>0.19</v>
+      </c>
+      <c r="O55">
+        <v>4.0999999999999995E-2</v>
+      </c>
+      <c r="P55">
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="V55">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="W55">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="AD55">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="AE55">
+        <v>0.05</v>
+      </c>
+      <c r="AF55">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" t="s">
+        <v>91</v>
+      </c>
+      <c r="D57">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="E57">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F57">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G57">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="H57">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="I57">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="J57">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="K57">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="L57">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Q57">
+        <v>2E-3</v>
+      </c>
+      <c r="R57">
+        <v>0.24</v>
+      </c>
+      <c r="S57">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="T57">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="U57">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="V57">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="W57">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="X57">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="Y57">
+        <f>SUM(V57,J57,O57)</f>
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="Z57">
+        <f>SUM(W57,K57,P57)</f>
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="AA57">
+        <f>SUM(S57,H57,M57)</f>
+        <v>0.96700000000000008</v>
+      </c>
+      <c r="AB57">
+        <f>SUM(T57,I57,N57)</f>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="AD57">
+        <v>0.54</v>
+      </c>
+      <c r="AE57">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AF57">
+        <v>0.14899999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" t="s">
+        <v>91</v>
+      </c>
+      <c r="J59">
+        <v>0.375</v>
+      </c>
+      <c r="K59">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O59">
+        <v>0.06</v>
+      </c>
+      <c r="P59">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="V59">
+        <v>0.214</v>
+      </c>
+      <c r="W59">
+        <v>0.112</v>
+      </c>
+      <c r="AD59">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="AE59">
+        <v>0.11</v>
+      </c>
+      <c r="AF59">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" t="s">
+        <v>143</v>
+      </c>
+      <c r="J60">
+        <v>0.10099999999999999</v>
+      </c>
+      <c r="K60">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="L60">
+        <v>0.23800000000000002</v>
+      </c>
+      <c r="O60">
+        <v>5.5E-2</v>
+      </c>
+      <c r="P60">
+        <v>0.113</v>
+      </c>
+      <c r="Q60">
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="V60">
+        <v>0.125</v>
+      </c>
+      <c r="W60">
+        <v>0.15400000000000003</v>
+      </c>
+      <c r="X60">
+        <v>0.14843098000000002</v>
+      </c>
+      <c r="Y60">
+        <f>SUM(V60,J60,O60)</f>
+        <v>0.28099999999999997</v>
+      </c>
+      <c r="Z60">
+        <f>SUM(W60,K60,P60)</f>
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="AD60">
+        <v>0.44098999999999999</v>
+      </c>
+      <c r="AE60">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AF60">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" t="s">
+        <v>143</v>
+      </c>
+      <c r="J61">
+        <v>5.9000000000000004E-2</v>
+      </c>
+      <c r="K61">
+        <v>0.105</v>
+      </c>
+      <c r="L61">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="O61">
+        <v>4.9937230000000003E-3</v>
+      </c>
+      <c r="P61">
+        <v>7.9606520000000004E-3</v>
+      </c>
+      <c r="Q61">
+        <v>2E-3</v>
+      </c>
+      <c r="V61">
+        <v>0.253</v>
+      </c>
+      <c r="W61">
+        <v>0.25</v>
+      </c>
+      <c r="X61">
+        <v>0.25089694000000001</v>
+      </c>
+      <c r="Y61">
+        <f>SUM(V61,J61,O61)</f>
+        <v>0.31699372300000001</v>
+      </c>
+      <c r="Z61">
+        <f>SUM(W61,K61,P61)</f>
+        <v>0.36296065199999999</v>
+      </c>
+      <c r="AD61">
+        <v>0.12044000000000001</v>
+      </c>
+      <c r="AE61">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AF61">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D62">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="E62">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="F62">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="G62">
+        <v>0.42100000000000004</v>
+      </c>
+      <c r="J62">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="K62">
+        <v>9.5500000000000002E-2</v>
+      </c>
+      <c r="L62">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="O62">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="P62">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q62">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="V62">
+        <v>0.128</v>
+      </c>
+      <c r="W62">
+        <v>0.28220000000000001</v>
+      </c>
+      <c r="X62">
+        <v>0.25629999999999997</v>
+      </c>
+      <c r="Y62">
+        <v>0.152</v>
+      </c>
+      <c r="Z62">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="AD62">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="AE62">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="AF62">
+        <v>0.22899999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="E63">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="F63">
+        <v>0.247</v>
+      </c>
+      <c r="G63">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="H63">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="I63">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="J63">
+        <v>0.13313556252904693</v>
+      </c>
+      <c r="K63">
+        <v>0.29855396733462469</v>
+      </c>
+      <c r="L63">
+        <v>0.24709742861978748</v>
+      </c>
+      <c r="M63">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N63">
+        <v>0.128</v>
+      </c>
+      <c r="O63">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="P63">
+        <v>5.2000000000000005E-2</v>
+      </c>
+      <c r="Q63">
+        <v>3.9E-2</v>
+      </c>
+      <c r="R63">
+        <v>0.245</v>
+      </c>
+      <c r="S63">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="T63">
+        <v>0.21600000000000003</v>
+      </c>
+      <c r="U63">
+        <v>0.311</v>
+      </c>
+      <c r="V63">
+        <v>0.23</v>
+      </c>
+      <c r="W63">
+        <v>0.22699999999999998</v>
+      </c>
+      <c r="X63">
+        <v>0.22816478772845539</v>
+      </c>
+      <c r="Y63">
+        <v>0.377</v>
+      </c>
+      <c r="Z63">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="AA63">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="AB63">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="AD63">
+        <v>0.32</v>
+      </c>
+      <c r="AE63">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="AF63">
+        <v>0.221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" t="s">
+        <v>91</v>
+      </c>
+      <c r="D64">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="E64">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="F64">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="G64">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="J64">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="K64">
+        <v>0.187</v>
+      </c>
+      <c r="L64">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="O64">
+        <v>2.3E-2</v>
+      </c>
+      <c r="P64">
+        <v>1.4E-2</v>
+      </c>
+      <c r="Q64">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R64">
+        <v>0.747</v>
+      </c>
+      <c r="V64">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="W64">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="X64">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="Y64">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="Z64">
+        <v>0.49</v>
+      </c>
+      <c r="AD64">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="AE64">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AF64">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="65" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D65">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="E65">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F65">
+        <v>0.191</v>
+      </c>
+      <c r="G65">
+        <v>0.47</v>
+      </c>
+      <c r="H65">
+        <v>0.36</v>
+      </c>
+      <c r="I65">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="J65">
+        <v>7.6582433237668321E-2</v>
+      </c>
+      <c r="K65">
+        <v>0.15310923038945096</v>
+      </c>
+      <c r="L65">
+        <v>0.13818621731970959</v>
+      </c>
+      <c r="M65">
+        <v>5.5E-2</v>
+      </c>
+      <c r="N65">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="O65">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="P65">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="Q65">
+        <v>1.9E-2</v>
+      </c>
+      <c r="R65">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="S65">
+        <v>0.53299999999999992</v>
+      </c>
+      <c r="T65">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="U65">
+        <v>0.436</v>
+      </c>
+      <c r="V65">
+        <v>0.41600000000000004</v>
+      </c>
+      <c r="W65">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="X65">
+        <v>0.40040631676016059</v>
+      </c>
+      <c r="Y65">
+        <v>0.5</v>
+      </c>
+      <c r="Z65">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AA65">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AB65">
+        <v>0.85400000000000009</v>
+      </c>
+      <c r="AC65">
+        <v>0.59200000000000008</v>
+      </c>
+      <c r="AD65">
+        <v>0.17300000000000001</v>
+      </c>
+      <c r="AE65">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="AF65">
+        <v>0.33600000000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D66">
+        <v>0.54299999999999993</v>
+      </c>
+      <c r="E66">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F66">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="G66">
+        <v>0.57200000000000006</v>
+      </c>
+      <c r="H66">
+        <v>0.40299999999999997</v>
+      </c>
+      <c r="I66">
+        <v>0.501</v>
+      </c>
+      <c r="J66">
+        <v>0.20649999999999999</v>
+      </c>
+      <c r="K66">
+        <v>0.311</v>
+      </c>
+      <c r="L66">
+        <v>0.2838</v>
+      </c>
+      <c r="M66">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N66">
+        <v>5.5E-2</v>
+      </c>
+      <c r="O66">
+        <v>1.2E-2</v>
+      </c>
+      <c r="P66">
+        <v>2.92E-2</v>
+      </c>
+      <c r="Q66">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="R66">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="S66">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="T66">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="U66">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="V66">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="W66">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="X66">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="Y66">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="Z66">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="AA66">
+        <v>0.877</v>
+      </c>
+      <c r="AB66">
+        <v>0.82</v>
+      </c>
+      <c r="AC66">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="AD66">
+        <v>0.34760000000000002</v>
+      </c>
+      <c r="AE66">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="AF66">
+        <v>0.24399999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <f t="shared" ref="A68:A72" si="1">A67+1</f>
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>66</v>
+      </c>
+      <c r="J69" t="s">
+        <v>89</v>
+      </c>
+      <c r="K69" t="s">
+        <v>89</v>
+      </c>
+      <c r="L69" t="s">
+        <v>89</v>
+      </c>
+      <c r="V69" t="s">
+        <v>89</v>
+      </c>
+      <c r="W69" t="s">
+        <v>89</v>
+      </c>
+      <c r="X69" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" t="s">
+        <v>92</v>
+      </c>
+      <c r="J70">
+        <v>0.12080567759481116</v>
+      </c>
+      <c r="K70">
+        <v>0.22957959278865747</v>
+      </c>
+      <c r="L70">
+        <v>0.20048704262317799</v>
+      </c>
+      <c r="O70">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="P70">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Q70">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="V70">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="W70">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="X70">
+        <v>0.29319116756905994</v>
+      </c>
+      <c r="Y70">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="Z70">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="AD70">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="AE70">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AF70">
+        <v>0.28699999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" t="s">
+        <v>93</v>
+      </c>
+      <c r="J71">
+        <v>0.378</v>
+      </c>
+      <c r="K71">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="O71">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P71">
+        <v>1.2E-2</v>
+      </c>
+      <c r="V71">
+        <v>0.215</v>
+      </c>
+      <c r="W71">
+        <v>0.193</v>
+      </c>
+      <c r="Y71">
+        <f>SUM(V71,J71,O71)</f>
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="Z71">
+        <f>SUM(W71,K71,P71)</f>
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="AD71">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AE71">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="AF71">
+        <v>0.191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" t="s">
+        <v>78</v>
+      </c>
+      <c r="D72">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="E72">
+        <v>0.16</v>
+      </c>
+      <c r="F72">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="G72">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="H72">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="I72">
+        <v>0.69400000000000006</v>
+      </c>
+      <c r="J72">
+        <v>0.44926470122462042</v>
+      </c>
+      <c r="K72">
+        <v>0.6382048902980203</v>
+      </c>
+      <c r="L72">
+        <v>0.58299011459260852</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>1.2E-2</v>
+      </c>
+      <c r="O72">
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="P72">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q72">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="R72">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="S72">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="T72">
+        <v>0.16699999999999998</v>
+      </c>
+      <c r="U72">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="V72">
+        <v>0.126</v>
+      </c>
+      <c r="W72">
+        <v>0.10099999999999999</v>
+      </c>
+      <c r="X72">
+        <v>0.10806876517923798</v>
+      </c>
+      <c r="Y72">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="Z72">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="AA72">
+        <v>0.78299999999999992</v>
+      </c>
+      <c r="AB72">
+        <v>0.873</v>
+      </c>
+      <c r="AC72">
+        <v>0.442</v>
+      </c>
+      <c r="AD72">
+        <v>0.65799999999999992</v>
+      </c>
+      <c r="AE72">
+        <v>0.01</v>
+      </c>
+      <c r="AF72">
+        <v>0.10400000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF80" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>